<commit_message>
constructor indicators | qualifier
</commit_message>
<xml_diff>
--- a/data/drv_ctr_qualifier.xlsx
+++ b/data/drv_ctr_qualifier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diiim\Documents\job_uni\Master\Thesis\F1_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE40659-C237-497F-B565-6D2676BD1B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6A501C-2242-4589-9755-670A56FC1269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3481" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3481" uniqueCount="230">
   <si>
     <t>driver</t>
   </si>
@@ -715,9 +715,6 @@
   </si>
   <si>
     <t>mazepin</t>
-  </si>
-  <si>
-    <t>ctr t0</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1086,7 @@
   <dimension ref="A1:FE52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="FE1" sqref="FE1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1099,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>230</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>

</xml_diff>